<commit_message>
Envio inicial do projeto
</commit_message>
<xml_diff>
--- a/data/cnpjs_test.xlsx
+++ b/data/cnpjs_test.xlsx
@@ -113,13 +113,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -139,13 +143,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.85"/>
   </cols>
@@ -157,8 +161,11 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>15374076</v>
+        <v>26290626</v>
       </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>